<commit_message>
towards new measurement integration
</commit_message>
<xml_diff>
--- a/data/2021_waters_collection.xlsx
+++ b/data/2021_waters_collection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emojifilesystem/RND/Turkana/waters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emojifilesystem/RND/Turkana-waters/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17F485DD-F53E-6344-90EC-E94A03A3E366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EAB194-40F7-F744-A630-995B096A1B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="1120" windowWidth="27240" windowHeight="16040" xr2:uid="{CB9AB020-742B-B44E-97E5-4540017A25E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>SampleID</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>MSTW-21-18</t>
+  </si>
+  <si>
+    <t>3'08.520</t>
+  </si>
+  <si>
+    <t>35'51.722</t>
+  </si>
+  <si>
+    <t>3'08.521</t>
+  </si>
+  <si>
+    <t>35'51.723</t>
   </si>
 </sst>
 </file>
@@ -583,7 +595,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,6 +906,12 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
       <c r="H12">
         <v>30.6</v>
       </c>
@@ -914,6 +932,12 @@
       <c r="E13" t="s">
         <v>50</v>
       </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -931,6 +955,12 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -951,7 +981,7 @@
       <c r="F15" s="3">
         <v>2.9352</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <v>36.059339999999999</v>
       </c>
       <c r="H15">
@@ -974,10 +1004,10 @@
       <c r="E16" t="s">
         <v>55</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>2.9414099999999999</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>36.02807</v>
       </c>
     </row>
@@ -997,10 +1027,10 @@
       <c r="E17" t="s">
         <v>58</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>2.8966099999999999</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>36.063580000000002</v>
       </c>
     </row>
@@ -1020,10 +1050,10 @@
       <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>2.9274499999999999</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>36.058070000000001</v>
       </c>
     </row>
@@ -1042,6 +1072,12 @@
       </c>
       <c r="E19" t="s">
         <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>